<commit_message>
before changes in test structure
</commit_message>
<xml_diff>
--- a/hyperareas.xlsx
+++ b/hyperareas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
   <si>
     <t>population</t>
   </si>
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,7 +411,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.3661306432443686</v>
+        <v>0.3285138811888638</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -425,7 +425,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.3213563175310605</v>
+        <v>0.3216747188243654</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -439,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.3512022270136961</v>
+        <v>0.3286024557405686</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -453,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0.3235623632297607</v>
+        <v>0.3211807332839862</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.363188498510129</v>
+        <v>0.3288331149508074</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -481,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>0.3225472349590994</v>
+        <v>0.3219496020622352</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.3633936299512332</v>
+        <v>0.3285318265659036</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>0.3228581648980274</v>
+        <v>0.3224131462840029</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -523,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0.3542395658070417</v>
+        <v>0.3287359510336123</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <v>0.3176772509895869</v>
+        <v>0.3230641013449289</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0.360022763082824</v>
+        <v>0.3286534576049262</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -565,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>0.3213492682088243</v>
+        <v>0.3240327853785042</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -579,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>0.3598556544864012</v>
+        <v>0.3287990759682234</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -593,66 +593,10 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>0.3226817198378662</v>
+        <v>0.3201716152902284</v>
       </c>
       <c r="D15">
         <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>0.344578339890963</v>
-      </c>
-      <c r="D16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>0.3223468820121568</v>
-      </c>
-      <c r="D17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>0.3602575758573314</v>
-      </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>0.3187032174270185</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>